<commit_message>
Analysis for PSC statistics in an opto dataset
as title
</commit_message>
<xml_diff>
--- a/result_table_templates/PostSynapticCurrent.xlsx
+++ b/result_table_templates/PostSynapticCurrent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\githubRepos\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE820E2-F17A-436C-87E1-98B74FDA21EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E856BA3E-5568-41F3-BD35-C7AA11FAAA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{6798E00C-8699-40E6-8FEF-DDE56C0B6C6C}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{6798E00C-8699-40E6-8FEF-DDE56C0B6C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,27 +74,18 @@
     <t>cell</t>
   </si>
   <si>
-    <t>rise time of the PSC in milisecods</t>
-  </si>
-  <si>
     <t>sample_rate</t>
   </si>
   <si>
     <t>sampling rate of this recording</t>
   </si>
   <si>
-    <t>decay time of the PSC in miliseconds</t>
-  </si>
-  <si>
     <t>total number of the detected PSC</t>
   </si>
   <si>
     <t xml:space="preserve">the vector denoting the peak amplitude of PSC </t>
   </si>
   <si>
-    <t>the vector denoting the starting time of PSC in miliseconds</t>
-  </si>
-  <si>
     <t>psc_start_ms</t>
   </si>
   <si>
@@ -108,6 +99,15 @@
   </si>
   <si>
     <t>psc_total</t>
+  </si>
+  <si>
+    <t>rise time of the PSC in secods</t>
+  </si>
+  <si>
+    <t>decay time of the PSC in seconds</t>
+  </si>
+  <si>
+    <t>the vector denoting the starting time of PSC in seconds</t>
   </si>
 </sst>
 </file>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DD6D41-705F-45B8-AF11-3673F73A490D}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -525,13 +525,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
@@ -547,57 +547,57 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed unit bug in psc detection scripts
</commit_message>
<xml_diff>
--- a/result_table_templates/PostSynapticCurrent.xlsx
+++ b/result_table_templates/PostSynapticCurrent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\githubRepos\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E856BA3E-5568-41F3-BD35-C7AA11FAAA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ED5F84-7EE7-4F0E-855A-7032938DB38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{6798E00C-8699-40E6-8FEF-DDE56C0B6C6C}"/>
   </bookViews>
@@ -101,13 +101,13 @@
     <t>psc_total</t>
   </si>
   <si>
-    <t>rise time of the PSC in secods</t>
-  </si>
-  <si>
-    <t>decay time of the PSC in seconds</t>
-  </si>
-  <si>
-    <t>the vector denoting the starting time of PSC in seconds</t>
+    <t>the vector denoting the starting time of PSC in miliseconds</t>
+  </si>
+  <si>
+    <t>rise time of the PSC in milisecods</t>
+  </si>
+  <si>
+    <t>decay time of the PSC in miliseconds</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -553,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
@@ -575,7 +575,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.75">
@@ -586,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.75">

</xml_diff>